<commit_message>
claude, with own corrections
</commit_message>
<xml_diff>
--- a/testdata/invalid-testdata/excel2json/json_header_empty_sheet.xlsx
+++ b/testdata/invalid-testdata/excel2json/json_header_empty_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/invalid-testdata/excel2json/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/testdata/invalid-testdata/excel2json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF307F9C-DE37-4943-B48A-3F6D0B6A6A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDBD9FD-7F1E-7841-81C9-4FF4A2C4E887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="21880" windowWidth="25540" windowHeight="9000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,19 @@
     <sheet name="Keywords" sheetId="4" r:id="rId4"/>
     <sheet name="Users" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="eXIUItnczbsgwU2bhTxsCIaPyk1rdouaLJcS/mum0so="/>
     </ext>
@@ -29,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>prefixes</t>
   </si>
@@ -161,6 +172,12 @@
   </si>
   <si>
     <t>this does not count as a row</t>
+  </si>
+  <si>
+    <t>project_default_permissions</t>
+  </si>
+  <si>
+    <t>public</t>
   </si>
 </sst>
 </file>
@@ -1561,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1584,7 +1601,9 @@
       <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1618,7 +1637,9 @@
       <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
@@ -6618,7 +6639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat(excel2json): set project default permissions in Excel (DEV-5036) (#1808)
</commit_message>
<xml_diff>
--- a/testdata/invalid-testdata/excel2json/json_header_empty_sheet.xlsx
+++ b/testdata/invalid-testdata/excel2json/json_header_empty_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/invalid-testdata/excel2json/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/testdata/invalid-testdata/excel2json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF307F9C-DE37-4943-B48A-3F6D0B6A6A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDBD9FD-7F1E-7841-81C9-4FF4A2C4E887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="21880" windowWidth="25540" windowHeight="9000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,19 @@
     <sheet name="Keywords" sheetId="4" r:id="rId4"/>
     <sheet name="Users" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="eXIUItnczbsgwU2bhTxsCIaPyk1rdouaLJcS/mum0so="/>
     </ext>
@@ -29,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>prefixes</t>
   </si>
@@ -161,6 +172,12 @@
   </si>
   <si>
     <t>this does not count as a row</t>
+  </si>
+  <si>
+    <t>project_default_permissions</t>
+  </si>
+  <si>
+    <t>public</t>
   </si>
 </sst>
 </file>
@@ -1561,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1584,7 +1601,9 @@
       <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1618,7 +1637,9 @@
       <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
@@ -6618,7 +6639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>